<commit_message>
automate for all factsheets
</commit_message>
<xml_diff>
--- a/gqg_factsheet_gics_ranked_format.xlsx
+++ b/gqg_factsheet_gics_ranked_format.xlsx
@@ -14,11 +14,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="123">
   <si>
     <t>Rank</t>
   </si>
   <si>
+    <t>Jun 2024_Month</t>
+  </si>
+  <si>
+    <t>Jun 2024_Company</t>
+  </si>
+  <si>
+    <t>Jun 2024_Holding %</t>
+  </si>
+  <si>
     <t>Aug 2024_Month</t>
   </si>
   <si>
@@ -91,253 +100,289 @@
     <t>Jul 2025_Holding %</t>
   </si>
   <si>
+    <t>Jun 2024</t>
+  </si>
+  <si>
+    <t>Info Tech</t>
+  </si>
+  <si>
+    <t>Comm Serv</t>
+  </si>
+  <si>
+    <t>Health Care</t>
+  </si>
+  <si>
+    <t>Cons Stap</t>
+  </si>
+  <si>
+    <t>Utilities</t>
+  </si>
+  <si>
+    <t>Cons Disc</t>
+  </si>
+  <si>
+    <t>Financials</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>Real Estate</t>
+  </si>
+  <si>
+    <t>38.0%</t>
+  </si>
+  <si>
+    <t>15.8%</t>
+  </si>
+  <si>
+    <t>13.3%</t>
+  </si>
+  <si>
+    <t>11.0%</t>
+  </si>
+  <si>
+    <t>8.4%</t>
+  </si>
+  <si>
+    <t>4.7%</t>
+  </si>
+  <si>
+    <t>3.9%</t>
+  </si>
+  <si>
+    <t>2.8%</t>
+  </si>
+  <si>
+    <t>2.1%</t>
+  </si>
+  <si>
+    <t>-2.1%</t>
+  </si>
+  <si>
     <t>Aug 2024</t>
   </si>
   <si>
-    <t>Health Care</t>
-  </si>
-  <si>
-    <t>Info Tech</t>
-  </si>
-  <si>
-    <t>Comm Serv</t>
-  </si>
-  <si>
-    <t>Utilities</t>
-  </si>
-  <si>
-    <t>Energy</t>
-  </si>
-  <si>
-    <t>Financials</t>
-  </si>
-  <si>
-    <t>Cons Stap</t>
-  </si>
-  <si>
-    <t>Cash</t>
-  </si>
-  <si>
-    <t>Cons Disc</t>
+    <t>Materials</t>
+  </si>
+  <si>
+    <t>31.2%</t>
+  </si>
+  <si>
+    <t>17.2%</t>
+  </si>
+  <si>
+    <t>13.4%</t>
+  </si>
+  <si>
+    <t>11.3%</t>
+  </si>
+  <si>
+    <t>9.8%</t>
+  </si>
+  <si>
+    <t>8.8%</t>
+  </si>
+  <si>
+    <t>3.4%</t>
+  </si>
+  <si>
+    <t>2.6%</t>
+  </si>
+  <si>
+    <t>2.2%</t>
+  </si>
+  <si>
+    <t>-2.2%</t>
+  </si>
+  <si>
+    <t>Dec 2024</t>
   </si>
   <si>
     <t>Industrials</t>
   </si>
   <si>
-    <t>25.5%</t>
-  </si>
-  <si>
-    <t>16.4%</t>
-  </si>
-  <si>
-    <t>11.6%</t>
-  </si>
-  <si>
-    <t>10.6%</t>
-  </si>
-  <si>
-    <t>8.4%</t>
-  </si>
-  <si>
-    <t>7.9%</t>
-  </si>
-  <si>
-    <t>7.3%</t>
-  </si>
-  <si>
-    <t>6.0%</t>
+    <t>23.6%</t>
+  </si>
+  <si>
+    <t>22.0%</t>
+  </si>
+  <si>
+    <t>21.7%</t>
+  </si>
+  <si>
+    <t>12.0%</t>
+  </si>
+  <si>
+    <t>6.2%</t>
+  </si>
+  <si>
+    <t>3.7%</t>
+  </si>
+  <si>
+    <t>3.6%</t>
+  </si>
+  <si>
+    <t>2.9%</t>
+  </si>
+  <si>
+    <t>1.4%</t>
+  </si>
+  <si>
+    <t>Feb 2025</t>
+  </si>
+  <si>
+    <t>26.0%</t>
+  </si>
+  <si>
+    <t>23.8%</t>
+  </si>
+  <si>
+    <t>15.4%</t>
+  </si>
+  <si>
+    <t>11.1%</t>
+  </si>
+  <si>
+    <t>5.3%</t>
+  </si>
+  <si>
+    <t>5.0%</t>
+  </si>
+  <si>
+    <t>4.8%</t>
+  </si>
+  <si>
+    <t>Mar 2025</t>
+  </si>
+  <si>
+    <t>23.2%</t>
+  </si>
+  <si>
+    <t>16.3%</t>
+  </si>
+  <si>
+    <t>14.3%</t>
+  </si>
+  <si>
+    <t>13.0%</t>
+  </si>
+  <si>
+    <t>10.8%</t>
+  </si>
+  <si>
+    <t>9.7%</t>
+  </si>
+  <si>
+    <t>5.2%</t>
   </si>
   <si>
     <t>2.5%</t>
   </si>
   <si>
-    <t>Dec 2024</t>
-  </si>
-  <si>
-    <t>20.4%</t>
-  </si>
-  <si>
-    <t>19.0%</t>
+    <t>1.2%</t>
+  </si>
+  <si>
+    <t>Apr 2025</t>
+  </si>
+  <si>
+    <t>24.1%</t>
+  </si>
+  <si>
+    <t>20.0%</t>
   </si>
   <si>
     <t>16.5%</t>
   </si>
   <si>
-    <t>11.2%</t>
-  </si>
-  <si>
-    <t>9.2%</t>
-  </si>
-  <si>
-    <t>8.9%</t>
-  </si>
-  <si>
-    <t>4.1%</t>
-  </si>
-  <si>
-    <t>3.5%</t>
-  </si>
-  <si>
-    <t>3.2%</t>
-  </si>
-  <si>
-    <t>3.1%</t>
-  </si>
-  <si>
-    <t>Feb 2025</t>
-  </si>
-  <si>
-    <t>22.3%</t>
-  </si>
-  <si>
-    <t>20.8%</t>
+    <t>16.2%</t>
+  </si>
+  <si>
+    <t>7.1%</t>
+  </si>
+  <si>
+    <t>7.0%</t>
+  </si>
+  <si>
+    <t>3.8%</t>
+  </si>
+  <si>
+    <t>-2.0%</t>
+  </si>
+  <si>
+    <t>May 2025</t>
+  </si>
+  <si>
+    <t>22.2%</t>
+  </si>
+  <si>
+    <t>17.4%</t>
   </si>
   <si>
     <t>12.9%</t>
   </si>
   <si>
-    <t>12.3%</t>
+    <t>7.2%</t>
+  </si>
+  <si>
+    <t>6.5%</t>
+  </si>
+  <si>
+    <t>6.4%</t>
+  </si>
+  <si>
+    <t>-1.9%</t>
+  </si>
+  <si>
+    <t>Jun 2025</t>
+  </si>
+  <si>
+    <t>21.1%</t>
+  </si>
+  <si>
+    <t>19.7%</t>
+  </si>
+  <si>
+    <t>19.2%</t>
+  </si>
+  <si>
+    <t>16.8%</t>
   </si>
   <si>
     <t>9.5%</t>
   </si>
   <si>
-    <t>7.8%</t>
-  </si>
-  <si>
-    <t>4.9%</t>
-  </si>
-  <si>
-    <t>2.0%</t>
-  </si>
-  <si>
-    <t>Mar 2025</t>
-  </si>
-  <si>
-    <t>20.6%</t>
-  </si>
-  <si>
-    <t>15.0%</t>
-  </si>
-  <si>
-    <t>13.7%</t>
-  </si>
-  <si>
-    <t>12.7%</t>
-  </si>
-  <si>
-    <t>12.0%</t>
-  </si>
-  <si>
-    <t>6.8%</t>
-  </si>
-  <si>
-    <t>4.8%</t>
-  </si>
-  <si>
-    <t>1.7%</t>
-  </si>
-  <si>
-    <t>Apr 2025</t>
-  </si>
-  <si>
-    <t>16.6%</t>
-  </si>
-  <si>
-    <t>13.2%</t>
-  </si>
-  <si>
-    <t>9.8%</t>
-  </si>
-  <si>
-    <t>5.3%</t>
-  </si>
-  <si>
-    <t>0.8%</t>
-  </si>
-  <si>
-    <t>May 2025</t>
-  </si>
-  <si>
-    <t>22.5%</t>
-  </si>
-  <si>
-    <t>15.3%</t>
-  </si>
-  <si>
-    <t>13.4%</t>
-  </si>
-  <si>
-    <t>8.5%</t>
-  </si>
-  <si>
-    <t>7.2%</t>
-  </si>
-  <si>
-    <t>5.9%</t>
-  </si>
-  <si>
-    <t>3.9%</t>
-  </si>
-  <si>
-    <t>2.1%</t>
-  </si>
-  <si>
-    <t>Jun 2025</t>
-  </si>
-  <si>
-    <t>22.6%</t>
-  </si>
-  <si>
-    <t>20.1%</t>
-  </si>
-  <si>
-    <t>15.8%</t>
-  </si>
-  <si>
-    <t>10.3%</t>
-  </si>
-  <si>
-    <t>6.9%</t>
-  </si>
-  <si>
-    <t>3.6%</t>
-  </si>
-  <si>
-    <t>3.0%</t>
-  </si>
-  <si>
-    <t>1.1%</t>
+    <t>7.5%</t>
+  </si>
+  <si>
+    <t>1.5%</t>
+  </si>
+  <si>
+    <t>1.3%</t>
+  </si>
+  <si>
+    <t>0.0%</t>
   </si>
   <si>
     <t>Jul 2025</t>
   </si>
   <si>
-    <t>23.8%</t>
-  </si>
-  <si>
-    <t>23.1%</t>
-  </si>
-  <si>
-    <t>12.5%</t>
-  </si>
-  <si>
-    <t>10.0%</t>
-  </si>
-  <si>
-    <t>9.3%</t>
-  </si>
-  <si>
-    <t>7.0%</t>
-  </si>
-  <si>
-    <t>6.5%</t>
-  </si>
-  <si>
-    <t>4.2%</t>
-  </si>
-  <si>
-    <t>0.5%</t>
+    <t>22.7%</t>
+  </si>
+  <si>
+    <t>18.9%</t>
+  </si>
+  <si>
+    <t>18.4%</t>
+  </si>
+  <si>
+    <t>17.9%</t>
+  </si>
+  <si>
+    <t>8.2%</t>
   </si>
 </sst>
 </file>
@@ -695,13 +740,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y11"/>
+  <dimension ref="A1:AB11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:28">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -777,775 +822,874 @@
       <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:28">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="H2" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="I2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J2" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="K2" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="L2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M2" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="N2" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="O2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="P2" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="Q2" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="R2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="S2" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="T2" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="U2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="V2" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="W2" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="X2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="Y2" t="s">
-        <v>99</v>
+        <v>108</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:28">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G3" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="H3" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="I3" t="s">
         <v>31</v>
       </c>
       <c r="J3" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="K3" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="L3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" t="s">
+        <v>74</v>
+      </c>
+      <c r="N3" t="s">
+        <v>80</v>
+      </c>
+      <c r="O3" t="s">
         <v>30</v>
       </c>
-      <c r="M3" t="s">
-        <v>67</v>
-      </c>
-      <c r="N3" t="s">
-        <v>74</v>
-      </c>
-      <c r="O3" t="s">
-        <v>29</v>
-      </c>
       <c r="P3" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="Q3" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="R3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="S3" t="s">
-        <v>46</v>
+        <v>92</v>
       </c>
       <c r="T3" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="U3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="V3" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="W3" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="X3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Y3" t="s">
-        <v>100</v>
+        <v>109</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:28">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="H4" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="J4" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="K4" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="L4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="M4" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="N4" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="O4" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="P4" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="Q4" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="R4" t="s">
+        <v>31</v>
+      </c>
+      <c r="S4" t="s">
+        <v>93</v>
+      </c>
+      <c r="T4" t="s">
+        <v>99</v>
+      </c>
+      <c r="U4" t="s">
+        <v>30</v>
+      </c>
+      <c r="V4" t="s">
+        <v>101</v>
+      </c>
+      <c r="W4" t="s">
+        <v>107</v>
+      </c>
+      <c r="X4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA4" t="s">
         <v>32</v>
       </c>
-      <c r="S4" t="s">
-        <v>82</v>
-      </c>
-      <c r="T4" t="s">
-        <v>89</v>
-      </c>
-      <c r="U4" t="s">
-        <v>28</v>
-      </c>
-      <c r="V4" t="s">
-        <v>92</v>
-      </c>
-      <c r="W4" t="s">
-        <v>98</v>
-      </c>
-      <c r="X4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>101</v>
+      <c r="AB4" t="s">
+        <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:28">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" t="s">
+        <v>66</v>
+      </c>
+      <c r="K5" t="s">
+        <v>72</v>
+      </c>
+      <c r="L5" t="s">
         <v>29</v>
       </c>
-      <c r="D5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="M5" t="s">
+        <v>76</v>
+      </c>
+      <c r="N5" t="s">
+        <v>80</v>
+      </c>
+      <c r="O5" t="s">
+        <v>37</v>
+      </c>
+      <c r="P5" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>90</v>
+      </c>
+      <c r="R5" t="s">
+        <v>30</v>
+      </c>
+      <c r="S5" t="s">
+        <v>94</v>
+      </c>
+      <c r="T5" t="s">
+        <v>99</v>
+      </c>
+      <c r="U5" t="s">
         <v>31</v>
       </c>
-      <c r="G5" t="s">
-        <v>49</v>
-      </c>
-      <c r="H5" t="s">
-        <v>56</v>
-      </c>
-      <c r="I5" t="s">
-        <v>27</v>
-      </c>
-      <c r="J5" t="s">
-        <v>60</v>
-      </c>
-      <c r="K5" t="s">
-        <v>65</v>
-      </c>
-      <c r="L5" t="s">
-        <v>26</v>
-      </c>
-      <c r="M5" t="s">
-        <v>69</v>
-      </c>
-      <c r="N5" t="s">
-        <v>74</v>
-      </c>
-      <c r="O5" t="s">
-        <v>28</v>
-      </c>
-      <c r="P5" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>80</v>
-      </c>
-      <c r="R5" t="s">
-        <v>28</v>
-      </c>
-      <c r="S5" t="s">
-        <v>83</v>
-      </c>
-      <c r="T5" t="s">
-        <v>89</v>
-      </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
+        <v>102</v>
+      </c>
+      <c r="W5" t="s">
+        <v>107</v>
+      </c>
+      <c r="X5" t="s">
         <v>32</v>
       </c>
-      <c r="V5" t="s">
-        <v>93</v>
-      </c>
-      <c r="W5" t="s">
-        <v>98</v>
-      </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
+        <v>111</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA5" t="s">
         <v>30</v>
       </c>
-      <c r="Y5" t="s">
-        <v>102</v>
+      <c r="AB5" t="s">
+        <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:28">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G6" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="H6" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="I6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J6" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="K6" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="L6" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="M6" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="N6" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="O6" t="s">
+        <v>36</v>
+      </c>
+      <c r="P6" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>90</v>
+      </c>
+      <c r="R6" t="s">
         <v>32</v>
       </c>
-      <c r="P6" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>80</v>
-      </c>
-      <c r="R6" t="s">
-        <v>30</v>
-      </c>
       <c r="S6" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="T6" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="U6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="V6" t="s">
-        <v>50</v>
+        <v>103</v>
       </c>
       <c r="W6" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="X6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Y6" t="s">
-        <v>103</v>
+        <v>112</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:28">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G7" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="H7" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="I7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J7" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="K7" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="L7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="M7" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="N7" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="O7" t="s">
         <v>33</v>
       </c>
       <c r="P7" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="Q7" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="R7" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="S7" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="T7" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="U7" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="V7" t="s">
-        <v>42</v>
+        <v>104</v>
       </c>
       <c r="W7" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="X7" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="Y7" t="s">
-        <v>104</v>
+        <v>113</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:28">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E8" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F8" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G8" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="H8" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="I8" t="s">
+        <v>36</v>
+      </c>
+      <c r="J8" t="s">
+        <v>69</v>
+      </c>
+      <c r="K8" t="s">
+        <v>72</v>
+      </c>
+      <c r="L8" t="s">
+        <v>37</v>
+      </c>
+      <c r="M8" t="s">
+        <v>79</v>
+      </c>
+      <c r="N8" t="s">
+        <v>80</v>
+      </c>
+      <c r="O8" t="s">
         <v>29</v>
       </c>
-      <c r="J8" t="s">
-        <v>63</v>
-      </c>
-      <c r="K8" t="s">
-        <v>65</v>
-      </c>
-      <c r="L8" t="s">
-        <v>27</v>
-      </c>
-      <c r="M8" t="s">
-        <v>71</v>
-      </c>
-      <c r="N8" t="s">
-        <v>74</v>
-      </c>
-      <c r="O8" t="s">
-        <v>30</v>
-      </c>
       <c r="P8" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="Q8" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="R8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="S8" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="T8" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="U8" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="V8" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="W8" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="X8" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="Y8" t="s">
-        <v>105</v>
+        <v>57</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:28">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" t="s">
+        <v>61</v>
+      </c>
+      <c r="I9" t="s">
         <v>32</v>
       </c>
-      <c r="G9" t="s">
-        <v>53</v>
-      </c>
-      <c r="H9" t="s">
-        <v>56</v>
-      </c>
-      <c r="I9" t="s">
-        <v>35</v>
-      </c>
       <c r="J9" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="K9" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="L9" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="M9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N9" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="O9" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="P9" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="Q9" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="R9" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="S9" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="T9" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="U9" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="V9" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="W9" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="X9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Y9" t="s">
-        <v>106</v>
+        <v>114</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:28">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E10" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G10" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="H10" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="I10" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="J10" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="K10" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="L10" t="s">
         <v>32</v>
       </c>
       <c r="M10" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="N10" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="O10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="P10" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="Q10" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="R10" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="S10" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="T10" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="U10" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="V10" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="W10" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="X10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Y10" t="s">
-        <v>96</v>
+        <v>115</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:28">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F11" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="G11" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="H11" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="I11" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="J11" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="K11" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="L11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M11" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="N11" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="O11" t="s">
         <v>34</v>
       </c>
       <c r="P11" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="Q11" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="R11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="S11" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="T11" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="U11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="V11" t="s">
-        <v>97</v>
+        <v>48</v>
       </c>
       <c r="W11" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="X11" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="Y11" t="s">
-        <v>107</v>
+        <v>116</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>